<commit_message>
Modify the test data and fix counting bug and error report bug
</commit_message>
<xml_diff>
--- a/TestData/taxTestXlsx.xlsx
+++ b/TestData/taxTestXlsx.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbwuguo\Documents\Visual Studio 2013\Projects\TaxImport\TaxImport.UnitTest\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\taxImport\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="620">
   <si>
     <t>Acount1</t>
   </si>
@@ -1881,6 +1881,9 @@
   </si>
   <si>
     <t>Account</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -2200,7 +2203,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D308"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2357,7 +2362,7 @@
         <v>291</v>
       </c>
       <c r="C11" t="s">
-        <v>281</v>
+        <v>619</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -2469,7 +2474,7 @@
         <v>299</v>
       </c>
       <c r="C19" t="s">
-        <v>281</v>
+        <v>619</v>
       </c>
       <c r="D19">
         <v>18</v>

</xml_diff>